<commit_message>
EVO-130 Ejercicios Cuadriceps Terminados
</commit_message>
<xml_diff>
--- a/Documentos/EJERCICIOS DEFINITIVOS/Cuadriceps/0 Cuadriceps Ejercicios.xlsx
+++ b/Documentos/EJERCICIOS DEFINITIVOS/Cuadriceps/0 Cuadriceps Ejercicios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Carlos\Paginas web\Páginas React\EvoltFit\Evoltfit-web\Documentos\EJERCICIOS DEFINITIVOS\Cuadriceps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CETI\7to Semestre\0 EvoltFit\Evoltfit-web\Documentos\EJERCICIOS DEFINITIVOS\Cuadriceps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895359C9-02B9-4453-91C6-2F1E008CA4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1CEE98-1781-4D37-B35E-84AF270E965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{9FF0EE0F-1A49-644D-862B-969E3605F98A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{9FF0EE0F-1A49-644D-862B-969E3605F98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="115">
   <si>
     <t>Nombre</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Este movimiento es uno de los ejercicios más difíciles incluso para los atletas avanzados, ya que todo el peso se carga en una pierna. Es un ejercicio avanzado con una sola pierna que requiere equilibrio y estabilidad en comparación con la sentadilla estándar. Como ejercicio para la parte inferior del cuerpo, fortalece los músculos de las piernas, incluidos los cuádriceps, isquiotibiales, glúteos y gemelos.</t>
   </si>
   <si>
-    <t>Una técnica correcta es muy importante en este ejercicio. Una técnica incorrecta de sentadillas puede provocar lesiones. Por este motivo, se recomienda que quienes se inicien en las sentadillas divididas búlgaras por primera vez comiencen con el peso corporal.</t>
-  </si>
-  <si>
     <t>Sentadilla Búlgara con Barra</t>
   </si>
   <si>
@@ -336,6 +333,54 @@
   </si>
   <si>
     <t>La sentadilla búlgara dividida es una versión de la sentadilla con una sola pierna en la que la pierna de atrás se eleva sobre un banco o una silla resistente. Al ser una sentadilla unilateral con una sola pierna, el ejercicio se centra más en los cuádriceps que otros movimientos compuestos similares de la parte inferior del cuerpo. También requiere mucho equilibrio y coordinación, lo que aumenta el compromiso del tronco y la parte superior del cuerpo para mantener la forma adecuada. Lo principal que hay que recordar sobre la sentadilla búlgara dividida es que se necesita un poco de ensayo y error para encontrar la colocación adecuada del pie para realizar el ejercicio cómodamente.</t>
+  </si>
+  <si>
+    <t>Leg Press a una Pierna</t>
+  </si>
+  <si>
+    <t>Sentadilla Frontal con Barra</t>
+  </si>
+  <si>
+    <t>SINGLE LEG PRESS</t>
+  </si>
+  <si>
+    <t>BARBELL FRONT SQUAT</t>
+  </si>
+  <si>
+    <t>El leg press a una pierna es un tipo de ejercicio de entrenamiento de fuerza. Es un movimiento eficaz para fortalecer los cuádriceps, que se encuentran en la parte delantera de la parte superior de las piernas. Si tienes un desequilibrio muscular o una pierna es más débil que la otra, la prensa con una sola pierna es un ejercicio aislado unilateral que se utiliza para desarrollar los músculos de las piernas.</t>
+  </si>
+  <si>
+    <t>La Sentadilla Frontal (Front Squat) es una variante de Sentadillas que en los últimos años se ha difundido mayormente, sobre todo por medio del Crossfit: permite mantener el torso más vertical, mayor profundidad y mayor énfasis en los cuádriceps.</t>
+  </si>
+  <si>
+    <t>Procurar profundidad, evitar rodillas hacia adentro, procurar distribuir peso en los pies, evitar levantar los talones, procurar mantener la espalda recta y procurar tener los pies separados al ancho de los hombros.</t>
+  </si>
+  <si>
+    <t>Procurar profundidad, evitar rodillas hacia adentro, procurar distribuir peso en los pies, evitar levantar los talones, procurar mantener la espalda recta.</t>
+  </si>
+  <si>
+    <t>Evitar estrés en la rodilla, procurar movimiento lento y controlado, procurar rango de movimiento completo.</t>
+  </si>
+  <si>
+    <t>Evitar mala alineación, procurar buena estabilidad, procurar rango de movimiento completo, evitar sobrecarga de peso, procurar movimiento lento y controlado.</t>
+  </si>
+  <si>
+    <t>Procurar mantener una espalda recta, evitar pasos demasiado grandes, procurar rodillas alineadas, procurar estabilidad y control, evitar sobrecargar el peso y sacrificar técnica.</t>
+  </si>
+  <si>
+    <t>Evitar sobrecargar peso, evitar estirar piernas de mas, evitar presión en las rodillas, evitar inclinarse hacia adelante, procurar estar bien sentado en la maquina, procurar colocar correctamente los pies.</t>
+  </si>
+  <si>
+    <t>Procurar amortiguar el impacto, evitar movimientos bruscos, procurar buena postura, procurar coordinación.</t>
+  </si>
+  <si>
+    <t>Evitar inclinarse hacia adelante, procurar profundidad y rango de movimiento, procurar activación de abdomen, evitar exigir de mas a su movilidad y flexibilidad.</t>
+  </si>
+  <si>
+    <t>Evitar inclinarse hacia adelante, procurar estabilidad, procurar profundidad y rango de movimiento, procurar tener buena flexibilidad.</t>
+  </si>
+  <si>
+    <t>Procurar buena postura, procurar rango de movimiento completo, evitar utilizar impulso, procurar control y estabilidad en el movimiento.</t>
   </si>
 </sst>
 </file>
@@ -385,12 +430,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EF958E-4EEE-8244-B144-5B66B6AE234E}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G40" sqref="A31:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -733,7 +779,7 @@
     <col min="7" max="7" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5">
+    <row r="2" spans="1:8" ht="16.5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -770,13 +816,16 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -795,8 +844,11 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -812,8 +864,12 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -832,8 +888,11 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -852,8 +911,11 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -872,8 +934,11 @@
       <c r="F7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -892,8 +957,11 @@
       <c r="F8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -912,8 +980,11 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -932,8 +1003,11 @@
       <c r="F10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -952,10 +1026,13 @@
       <c r="F11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
@@ -972,10 +1049,13 @@
       <c r="F12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
@@ -993,15 +1073,15 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1013,18 +1093,18 @@
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -1036,15 +1116,18 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1056,15 +1139,18 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1076,15 +1162,18 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1096,15 +1185,18 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -1116,15 +1208,18 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -1136,15 +1231,18 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
@@ -1156,15 +1254,18 @@
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>73</v>
+      </c>
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
         <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1176,15 +1277,18 @@
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>73</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1196,15 +1300,18 @@
         <v>16</v>
       </c>
       <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1213,18 +1320,21 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>85</v>
       </c>
-      <c r="F24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -1233,18 +1343,21 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>86</v>
+      </c>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -1253,18 +1366,21 @@
         <v>6</v>
       </c>
       <c r="E26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" t="s">
         <v>91</v>
       </c>
-      <c r="F26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
@@ -1276,15 +1392,18 @@
         <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>93</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
@@ -1293,70 +1412,59 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4">
-      <c r="D40" t="s">
-        <v>6</v>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1366,6 +1474,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>